<commit_message>
corrigindo a memória e começando o assembler
</commit_message>
<xml_diff>
--- a/M68000/documentation/commands.xlsx
+++ b/M68000/documentation/commands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="91">
   <si>
     <t>Instruciton</t>
   </si>
@@ -248,44 +248,6 @@
   </si>
   <si>
     <t>Immediate Data V Destination ® Destination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Shift Operation</t>
-  </si>
-  <si>
-    <t>ASL</t>
-  </si>
-  <si>
-    <t>LSL</t>
-  </si>
-  <si>
-    <t>SWAP</t>
-  </si>
-  <si>
-    <t>Dn, Dn
-# data , Dn
-&lt;ea&gt;</t>
-  </si>
-  <si>
-    <t>BFCHG</t>
-  </si>
-  <si>
-    <t>BFCLR</t>
-  </si>
-  <si>
-    <t>BFSET</t>
-  </si>
-  <si>
-    <t>&lt;ea&gt; {offset:width}</t>
-  </si>
-  <si>
-    <t>0's -&gt; Field</t>
-  </si>
-  <si>
-    <t>~ Field -&gt; Field</t>
-  </si>
-  <si>
-    <t>1's -&gt; Field</t>
   </si>
   <si>
     <t xml:space="preserve">      Program Control Operation</t>
@@ -454,8 +416,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -531,6 +497,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -540,14 +512,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -567,6 +533,8 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -586,148 +554,13 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3086100</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>736600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Screen Shot 2014-11-22 at 3.50.23 PM.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2603500" y="11277600"/>
-          <a:ext cx="3035300" cy="685800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3048000</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>609600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="Screen Shot 2014-11-22 at 3.51.21 PM.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2616200" y="12039600"/>
-          <a:ext cx="2984500" cy="571500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1689100</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>901700</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="Screen Shot 2014-11-22 at 3.52.28 PM.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2603500" y="12725400"/>
-          <a:ext cx="1638300" cy="850900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1052,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:C53"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1066,11 +899,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -1092,18 +925,18 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="28" customHeight="1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="42">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1118,7 +951,7 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="42">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1133,7 +966,7 @@
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="28">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1148,7 +981,7 @@
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="28">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1163,7 +996,7 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="28">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1178,7 +1011,7 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1193,7 +1026,7 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1208,7 +1041,7 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1223,7 +1056,7 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1238,7 +1071,7 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1253,7 +1086,7 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1268,7 +1101,7 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="42">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1283,7 +1116,7 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="42">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1298,7 +1131,7 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="13" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1313,7 +1146,7 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1328,7 +1161,7 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="42">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1343,7 +1176,7 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="42">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1358,7 +1191,7 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1373,7 +1206,7 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1388,7 +1221,7 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" ht="42">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1403,7 +1236,7 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="42">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1418,7 +1251,7 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1433,7 +1266,7 @@
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="13" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1448,7 +1281,7 @@
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" ht="28">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="13" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1463,18 +1296,18 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="28" customHeight="1">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="28">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="13" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1489,7 +1322,7 @@
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="13" t="s">
         <v>57</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1504,7 +1337,7 @@
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="13" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1519,7 +1352,7 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="13" t="s">
         <v>59</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1534,7 +1367,7 @@
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="13" t="s">
         <v>60</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1549,7 +1382,7 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" ht="28">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="13" t="s">
         <v>61</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -1564,7 +1397,7 @@
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="13" t="s">
         <v>62</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1579,195 +1412,154 @@
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" ht="28" customHeight="1">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" ht="61" customHeight="1">
-      <c r="A37" s="16" t="s">
+    <row r="37" spans="1:7">
+      <c r="A37" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="53" customHeight="1">
-      <c r="A38" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="8"/>
-    </row>
-    <row r="39" spans="1:7" ht="73" customHeight="1">
-      <c r="A39" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="8"/>
+      <c r="C39" s="10" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="28" customHeight="1">
-      <c r="A40" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
+      <c r="A40" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" s="2" t="s">
+    <row r="41" spans="1:7" ht="28">
+      <c r="A41" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="28">
+      <c r="A42" s="13" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>81</v>
+      <c r="B42" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="16" t="s">
-        <v>79</v>
+      <c r="A43" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="28" customHeight="1">
-      <c r="A44" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" s="10" t="s">
         <v>86</v>
       </c>
+      <c r="C43" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" ht="144" customHeight="1">
+      <c r="A45" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>101</v>
-      </c>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="10"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="28" customHeight="1">
-      <c r="A48" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:3" ht="28">
-      <c r="A49" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="28">
-      <c r="A50" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>96</v>
-      </c>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="10"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="11"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="11"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="11"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>99</v>
-      </c>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="11"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="10"/>
-    </row>
-    <row r="53" spans="1:3" ht="144" customHeight="1">
-      <c r="A53" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="11"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="11"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="10"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="11"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="10"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="11"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="5"/>
@@ -1802,65 +1594,22 @@
     <row r="62" spans="1:3">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
-      <c r="C62" s="11"/>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
-      <c r="C63" s="11"/>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="11"/>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="11"/>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="11"/>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="11"/>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="11"/>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="11"/>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A48:C48"/>
+  <mergeCells count="6">
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A44:C44"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Alterações referências dos Registradores
</commit_message>
<xml_diff>
--- a/M68000/documentation/commands.xlsx
+++ b/M68000/documentation/commands.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Documents\GitHub\virtualPC\M68000\documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15516" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
   <si>
     <t>Instruciton</t>
   </si>
@@ -332,12 +337,48 @@
 6 - Pode ser para a entregar uma semana a mais! u.u</t>
     </r>
   </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>00000110</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>00000010</t>
+  </si>
+  <si>
+    <t>0110</t>
+  </si>
+  <si>
+    <t>01100000</t>
+  </si>
+  <si>
+    <t>01000010</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>00001100</t>
+  </si>
+  <si>
+    <t>00000XX011</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -461,7 +502,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -512,54 +553,65 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -885,731 +937,783 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:C40"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="54.1640625" customWidth="1"/>
+    <col min="1" max="1" width="30.5" style="18" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="54.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:8" ht="22.8">
+      <c r="B1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="17"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="3"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="17">
-      <c r="A2" s="6" t="s">
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.399999999999999">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="28" customHeight="1">
-      <c r="A3" s="15" t="s">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="28.05" customHeight="1">
+      <c r="B3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="15"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="42">
-      <c r="A4" s="13" t="s">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="45">
+      <c r="A4" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="42">
-      <c r="A5" s="13" t="s">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="45">
+      <c r="A5" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="28">
-      <c r="A6" s="13" t="s">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="28">
-      <c r="A7" s="13" t="s">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="30">
+      <c r="A7" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" ht="28">
-      <c r="A8" s="13" t="s">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="30">
+      <c r="A8" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="13" t="s">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="13" t="s">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="13" t="s">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="13" t="s">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="13" t="s">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="13" t="s">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" ht="42">
-      <c r="A15" s="13" t="s">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="45">
+      <c r="A15" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" ht="42">
-      <c r="A16" s="13" t="s">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="45">
+      <c r="A16" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="13" t="s">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="B17" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="13" t="s">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="B18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" ht="42">
-      <c r="A19" s="13" t="s">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="45">
+      <c r="B19" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" ht="42">
-      <c r="A20" s="13" t="s">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="45">
+      <c r="B20" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="13" t="s">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="13" t="s">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="B22" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" ht="42">
-      <c r="A23" s="13" t="s">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="45">
+      <c r="B23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" ht="42">
-      <c r="A24" s="13" t="s">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" ht="45">
+      <c r="B24" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="13" t="s">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="B25" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="13" t="s">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" ht="28">
-      <c r="A27" s="13" t="s">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="30">
+      <c r="B27" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="D27" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" ht="28" customHeight="1">
-      <c r="A28" s="15" t="s">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="28.05" customHeight="1">
+      <c r="B28" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="15"/>
       <c r="C28" s="15"/>
-      <c r="D28" s="1"/>
+      <c r="D28" s="15"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" ht="28">
-      <c r="A29" s="13" t="s">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" ht="30">
+      <c r="A29" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="13" t="s">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="13" t="s">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="D31" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="13" t="s">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="B32" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="D32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="13" t="s">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="B33" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D33" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" ht="28">
-      <c r="A34" s="13" t="s">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" ht="30">
+      <c r="B34" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="13" t="s">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="B35" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="D35" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" ht="28" customHeight="1">
-      <c r="A36" s="15" t="s">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" ht="28.05" customHeight="1">
+      <c r="B36" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="15"/>
       <c r="C36" s="15"/>
-      <c r="D36" s="1"/>
+      <c r="D36" s="15"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="13" t="s">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="B37" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="D37" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="13" t="s">
+    <row r="38" spans="1:8">
+      <c r="A38" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="13" t="s">
+    <row r="39" spans="1:8">
+      <c r="A39" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="D39" s="10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="28" customHeight="1">
-      <c r="A40" s="15" t="s">
+    <row r="40" spans="1:8" ht="28.05" customHeight="1">
+      <c r="B40" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="15"/>
       <c r="C40" s="15"/>
-      <c r="D40" s="1"/>
+      <c r="D40" s="15"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" ht="28">
-      <c r="A41" s="13" t="s">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" ht="30">
+      <c r="B41" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="D41" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="28">
-      <c r="A42" s="13" t="s">
+    <row r="42" spans="1:8" ht="30">
+      <c r="B42" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="D42" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="13" t="s">
+    <row r="43" spans="1:8">
+      <c r="B43" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="D43" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="2"/>
+    <row r="44" spans="1:8">
       <c r="B44" s="2"/>
-      <c r="C44" s="10"/>
-    </row>
-    <row r="45" spans="1:7" ht="144" customHeight="1">
-      <c r="A45" s="14" t="s">
+      <c r="C44" s="2"/>
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:8" ht="144" customHeight="1">
+      <c r="B45" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B45" s="14"/>
       <c r="C45" s="14"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="2"/>
+      <c r="D45" s="14"/>
+    </row>
+    <row r="46" spans="1:8">
       <c r="B46" s="2"/>
-      <c r="C46" s="10"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="10"/>
+    </row>
+    <row r="47" spans="1:8">
       <c r="B47" s="2"/>
-      <c r="C47" s="10"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="5"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:8">
       <c r="B48" s="5"/>
-      <c r="C48" s="11"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="2:4">
       <c r="B49" s="5"/>
-      <c r="C49" s="11"/>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="11"/>
+    </row>
+    <row r="50" spans="2:4">
       <c r="B50" s="5"/>
-      <c r="C50" s="11"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="2:4">
       <c r="B51" s="5"/>
-      <c r="C51" s="11"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="2:4">
       <c r="B52" s="5"/>
-      <c r="C52" s="11"/>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="2:4">
       <c r="B53" s="5"/>
-      <c r="C53" s="11"/>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="11"/>
+    </row>
+    <row r="54" spans="2:4">
       <c r="B54" s="5"/>
-      <c r="C54" s="11"/>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="11"/>
+    </row>
+    <row r="55" spans="2:4">
       <c r="B55" s="5"/>
-      <c r="C55" s="11"/>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="11"/>
+    </row>
+    <row r="56" spans="2:4">
       <c r="B56" s="5"/>
-      <c r="C56" s="11"/>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="11"/>
+    </row>
+    <row r="57" spans="2:4">
       <c r="B57" s="5"/>
-      <c r="C57" s="11"/>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="11"/>
+    </row>
+    <row r="58" spans="2:4">
       <c r="B58" s="5"/>
-      <c r="C58" s="11"/>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="11"/>
+    </row>
+    <row r="59" spans="2:4">
       <c r="B59" s="5"/>
-      <c r="C59" s="11"/>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="11"/>
+    </row>
+    <row r="60" spans="2:4">
       <c r="B60" s="5"/>
-      <c r="C60" s="11"/>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="11"/>
+    </row>
+    <row r="61" spans="2:4">
       <c r="B61" s="5"/>
-      <c r="C61" s="11"/>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="11"/>
+    </row>
+    <row r="62" spans="2:4">
       <c r="B62" s="5"/>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="5"/>
+      <c r="C62" s="5"/>
+    </row>
+    <row r="63" spans="2:4">
       <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B36:D36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
ajustando para começar o linkador
</commit_message>
<xml_diff>
--- a/M68000/documentation/commands.xlsx
+++ b/M68000/documentation/commands.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Documents\GitHub\virtualPC\M68000\documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15516" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="126">
   <si>
     <t>Instruciton</t>
   </si>
@@ -373,12 +368,106 @@
   <si>
     <t>1000</t>
   </si>
+  <si>
+    <t>binary code</t>
+  </si>
+  <si>
+    <t>object code</t>
+  </si>
+  <si>
+    <t>01
+02
+03</t>
+  </si>
+  <si>
+    <t>04
+05
+06</t>
+  </si>
+  <si>
+    <t>17
+18
+19</t>
+  </si>
+  <si>
+    <t>20
+21
+22</t>
+  </si>
+  <si>
+    <t>25
+26
+27</t>
+  </si>
+  <si>
+    <t>28
+29
+30</t>
+  </si>
+  <si>
+    <t>33
+34
+35</t>
+  </si>
+  <si>
+    <t>36
+37
+38</t>
+  </si>
+  <si>
+    <t>41
+42</t>
+  </si>
+  <si>
+    <t>43
+44</t>
+  </si>
+  <si>
+    <t>49
+50</t>
+  </si>
+  <si>
+    <t>55
+56</t>
+  </si>
+  <si>
+    <t>57
+58</t>
+  </si>
+  <si>
+    <t>no
+no
+no</t>
+  </si>
+  <si>
+    <t>no
+no</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Assembler</t>
+  </si>
+  <si>
+    <t>Linker</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Implementated</t>
+  </si>
+  <si>
+    <t>09
+10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -396,12 +485,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="PetitaLight"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="PetitaLight"/>
     </font>
@@ -439,6 +522,18 @@
       <color theme="1"/>
       <name val="PetitaLight"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="PetitaLight"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="PetitaLight"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -457,52 +552,86 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -517,10 +646,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -538,8 +667,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -547,59 +679,109 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="42" builtinId="9" hidden="1"/>
+  <cellStyles count="77">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -937,783 +1119,1139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.5" style="18" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="54.19921875" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="14" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="54.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="22.8">
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:9" ht="24" customHeight="1">
+      <c r="A1" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="B1" s="17"/>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="17.399999999999999">
-      <c r="B2" s="6" t="s">
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="19">
+      <c r="A2" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="28.05" customHeight="1">
-      <c r="B3" s="15" t="s">
+      <c r="F2" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="28" customHeight="1">
+      <c r="A3" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="45">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="45">
       <c r="A4" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="45">
+      <c r="F4" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="45">
       <c r="A5" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="30">
-      <c r="A6" s="18" t="s">
+      <c r="F5" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="29">
+      <c r="A6" s="20">
+        <v>7</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="18" t="s">
+      <c r="F6" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="29">
+      <c r="A7" s="20">
+        <v>8</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="18" t="s">
+      <c r="F7" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="30">
+      <c r="A8" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="C8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="18" t="s">
+      <c r="F8" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="19">
+        <v>11</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="18" t="s">
+      <c r="F9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="19">
+        <v>12</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="C10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="18" t="s">
+      <c r="F10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="19">
+        <v>13</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="18" t="s">
+      <c r="F11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="19">
+        <v>14</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="C12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="18" t="s">
+      <c r="F12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="19">
+        <v>15</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="C13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="18" t="s">
+      <c r="F13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="19">
+        <v>16</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="C14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="45">
-      <c r="A15" s="18" t="s">
+      <c r="F14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="45">
+      <c r="A15" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="C15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="45">
-      <c r="A16" s="18" t="s">
+      <c r="F15" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="45">
+      <c r="A16" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="C16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="E16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="B17" s="13" t="s">
+      <c r="F16" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="19">
+        <v>23</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="B18" s="13" t="s">
+      <c r="F17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="19">
+        <v>24</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" ht="45">
-      <c r="B19" s="13" t="s">
+      <c r="F18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="45">
+      <c r="A19" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" ht="45">
-      <c r="B20" s="13" t="s">
+      <c r="F19" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" ht="45">
+      <c r="A20" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="E20" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="B21" s="13" t="s">
+      <c r="F20" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="19">
+        <v>31</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="B22" s="13" t="s">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="19">
+        <v>32</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" ht="45">
-      <c r="B23" s="13" t="s">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" ht="45">
+      <c r="A23" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" ht="45">
-      <c r="B24" s="13" t="s">
+      <c r="F23" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" ht="45">
+      <c r="A24" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="B25" s="13" t="s">
+      <c r="F24" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="19">
+        <v>39</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="B26" s="13" t="s">
+      <c r="F25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="19">
+        <v>40</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" ht="30">
-      <c r="B27" s="13" t="s">
+      <c r="F26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" ht="30">
+      <c r="A27" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" ht="28.05" customHeight="1">
-      <c r="B28" s="15" t="s">
+      <c r="F27" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" ht="28" customHeight="1">
+      <c r="A28" s="19"/>
+      <c r="C28" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" ht="30">
-      <c r="A29" s="18" t="s">
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" ht="30">
+      <c r="A29" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="C29" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="18" t="s">
+      <c r="F29" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="19">
+        <v>45</v>
+      </c>
+      <c r="B30" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="C30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="B31" s="13" t="s">
+      <c r="F30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="19">
+        <v>46</v>
+      </c>
+      <c r="C31" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E31" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="B32" s="13" t="s">
+      <c r="F31" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="19">
+        <v>47</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="B33" s="13" t="s">
+      <c r="F32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="19">
+        <v>48</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" ht="30">
-      <c r="B34" s="13" t="s">
+      <c r="F33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" ht="30">
+      <c r="A34" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="B35" s="13" t="s">
+      <c r="F34" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H34" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="19">
+        <v>51</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" ht="28.05" customHeight="1">
-      <c r="B36" s="15" t="s">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" ht="28" customHeight="1">
+      <c r="A36" s="19"/>
+      <c r="C36" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="1"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="B37" s="13" t="s">
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="19">
+        <v>52</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="E37" s="10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="18" t="s">
+      <c r="F37" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="19">
+        <v>53</v>
+      </c>
+      <c r="B38" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="C38" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="18" t="s">
+      <c r="F38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="19">
+        <v>54</v>
+      </c>
+      <c r="B39" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="C39" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="E39" s="10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="28.05" customHeight="1">
-      <c r="B40" s="15" t="s">
+      <c r="F39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="28" customHeight="1">
+      <c r="A40" s="19"/>
+      <c r="C40" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="1"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" ht="30">
-      <c r="B41" s="13" t="s">
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" ht="30">
+      <c r="A41" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="E41" s="12" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="30">
-      <c r="B42" s="13" t="s">
+      <c r="F41" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H41" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="30">
+      <c r="A42" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="E42" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="B43" s="13" t="s">
+      <c r="F42" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="G42" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H42" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="19">
+        <v>59</v>
+      </c>
+      <c r="C43" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="E43" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="B44" s="2"/>
+      <c r="F43" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="C44" s="2"/>
-      <c r="D44" s="10"/>
-    </row>
-    <row r="45" spans="1:8" ht="144" customHeight="1">
-      <c r="B45" s="14" t="s">
+      <c r="D44" s="2"/>
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="1:9" ht="144" customHeight="1">
+      <c r="C45" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="B46" s="2"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+    </row>
+    <row r="46" spans="1:9">
       <c r="C46" s="2"/>
-      <c r="D46" s="10"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="B47" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" spans="1:9">
       <c r="C47" s="2"/>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="B48" s="5"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="1:9">
       <c r="C48" s="5"/>
-      <c r="D48" s="11"/>
-    </row>
-    <row r="49" spans="2:4">
-      <c r="B49" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="11"/>
+    </row>
+    <row r="49" spans="3:5">
       <c r="C49" s="5"/>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="B50" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="11"/>
+    </row>
+    <row r="50" spans="3:5">
       <c r="C50" s="5"/>
-      <c r="D50" s="11"/>
-    </row>
-    <row r="51" spans="2:4">
-      <c r="B51" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="11"/>
+    </row>
+    <row r="51" spans="3:5">
       <c r="C51" s="5"/>
-      <c r="D51" s="11"/>
-    </row>
-    <row r="52" spans="2:4">
-      <c r="B52" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="11"/>
+    </row>
+    <row r="52" spans="3:5">
       <c r="C52" s="5"/>
-      <c r="D52" s="11"/>
-    </row>
-    <row r="53" spans="2:4">
-      <c r="B53" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="11"/>
+    </row>
+    <row r="53" spans="3:5">
       <c r="C53" s="5"/>
-      <c r="D53" s="11"/>
-    </row>
-    <row r="54" spans="2:4">
-      <c r="B54" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="11"/>
+    </row>
+    <row r="54" spans="3:5">
       <c r="C54" s="5"/>
-      <c r="D54" s="11"/>
-    </row>
-    <row r="55" spans="2:4">
-      <c r="B55" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="11"/>
+    </row>
+    <row r="55" spans="3:5">
       <c r="C55" s="5"/>
-      <c r="D55" s="11"/>
-    </row>
-    <row r="56" spans="2:4">
-      <c r="B56" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="11"/>
+    </row>
+    <row r="56" spans="3:5">
       <c r="C56" s="5"/>
-      <c r="D56" s="11"/>
-    </row>
-    <row r="57" spans="2:4">
-      <c r="B57" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="11"/>
+    </row>
+    <row r="57" spans="3:5">
       <c r="C57" s="5"/>
-      <c r="D57" s="11"/>
-    </row>
-    <row r="58" spans="2:4">
-      <c r="B58" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="11"/>
+    </row>
+    <row r="58" spans="3:5">
       <c r="C58" s="5"/>
-      <c r="D58" s="11"/>
-    </row>
-    <row r="59" spans="2:4">
-      <c r="B59" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="11"/>
+    </row>
+    <row r="59" spans="3:5">
       <c r="C59" s="5"/>
-      <c r="D59" s="11"/>
-    </row>
-    <row r="60" spans="2:4">
-      <c r="B60" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="11"/>
+    </row>
+    <row r="60" spans="3:5">
       <c r="C60" s="5"/>
-      <c r="D60" s="11"/>
-    </row>
-    <row r="61" spans="2:4">
-      <c r="B61" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="11"/>
+    </row>
+    <row r="61" spans="3:5">
       <c r="C61" s="5"/>
-      <c r="D61" s="11"/>
-    </row>
-    <row r="62" spans="2:4">
-      <c r="B62" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="11"/>
+    </row>
+    <row r="62" spans="3:5">
       <c r="C62" s="5"/>
-    </row>
-    <row r="63" spans="2:4">
-      <c r="B63" s="5"/>
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="3:5">
       <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B36:D36"/>
+  <mergeCells count="7">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
assembler funcionando interfaface ainda precisa de ajustes
</commit_message>
<xml_diff>
--- a/M68000/documentation/commands.xlsx
+++ b/M68000/documentation/commands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="130">
   <si>
     <t>Instruciton</t>
   </si>
@@ -461,6 +461,21 @@
   <si>
     <t>09
 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Operation</t>
+  </si>
+  <si>
+    <t>yes
+yes
+yes</t>
+  </si>
+  <si>
+    <t>yes
+yes</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -552,7 +567,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -630,8 +645,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -704,8 +723,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -744,6 +766,8 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -782,6 +806,8 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1121,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1175,13 +1201,13 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="28" customHeight="1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
       <c r="F3" s="24" t="s">
         <v>124</v>
       </c>
@@ -1206,7 +1232,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G4" s="23" t="s">
         <v>118</v>
@@ -1233,7 +1259,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G5" s="23" t="s">
         <v>118</v>
@@ -1260,7 +1286,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="G6" s="23" t="s">
         <v>119</v>
@@ -1270,7 +1296,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="29">
+    <row r="7" spans="1:9" ht="28">
       <c r="A7" s="20">
         <v>8</v>
       </c>
@@ -1287,13 +1313,13 @@
         <v>10</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -1341,7 +1367,7 @@
         <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>120</v>
@@ -2152,10 +2178,14 @@
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
     </row>
-    <row r="46" spans="1:9">
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="10"/>
+    <row r="46" spans="1:9" ht="27" customHeight="1">
+      <c r="A46" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
     </row>
     <row r="47" spans="1:9">
       <c r="C47" s="2"/>
@@ -2241,9 +2271,10 @@
       <c r="D63" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A46:E46"/>
     <mergeCell ref="C45:E45"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="C28:E28"/>

</xml_diff>

<commit_message>
Adicionando os últimos comandos
</commit_message>
<xml_diff>
--- a/M68000/documentation/commands.xlsx
+++ b/M68000/documentation/commands.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="133">
   <si>
     <t>Instruciton</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>Immediate Data -&gt; SR; STOP</t>
-  </si>
-  <si>
-    <t>Bcc</t>
   </si>
   <si>
     <t>If Condition True, Then PC + dn -&gt; PC</t>
@@ -476,6 +473,24 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>yes
+???
+no</t>
+  </si>
+  <si>
+    <t>yes
+??
+no</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
+    <t>yes
+no
+??</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1175,10 +1190,10 @@
     </row>
     <row r="2" spans="1:9" ht="19">
       <c r="A2" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>0</v>
@@ -1190,13 +1205,13 @@
         <v>2</v>
       </c>
       <c r="F2" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>122</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>123</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -1209,7 +1224,7 @@
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
       <c r="F3" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
@@ -1217,10 +1232,10 @@
     </row>
     <row r="4" spans="1:9" ht="45">
       <c r="A4" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
@@ -1232,22 +1247,22 @@
         <v>11</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="45">
       <c r="A5" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>4</v>
@@ -1259,13 +1274,13 @@
         <v>11</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -1274,7 +1289,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>6</v>
@@ -1286,13 +1301,13 @@
         <v>10</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -1301,7 +1316,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>7</v>
@@ -1313,22 +1328,22 @@
         <v>10</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="30">
       <c r="A8" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>8</v>
@@ -1340,13 +1355,13 @@
         <v>14</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -1355,7 +1370,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>15</v>
@@ -1367,13 +1382,13 @@
         <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -1382,7 +1397,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>18</v>
@@ -1394,13 +1409,13 @@
         <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I10" s="1"/>
     </row>
@@ -1409,7 +1424,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>19</v>
@@ -1421,13 +1436,13 @@
         <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -1436,7 +1451,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>20</v>
@@ -1448,13 +1463,13 @@
         <v>28</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -1463,7 +1478,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>21</v>
@@ -1475,13 +1490,13 @@
         <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I13" s="1"/>
     </row>
@@ -1490,7 +1505,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>22</v>
@@ -1502,22 +1517,22 @@
         <v>31</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="45">
       <c r="A15" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>23</v>
@@ -1529,22 +1544,22 @@
         <v>33</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="45">
       <c r="A16" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>24</v>
@@ -1556,13 +1571,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -1580,13 +1595,13 @@
         <v>37</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -1604,19 +1619,19 @@
         <v>37</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" ht="45">
       <c r="A19" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>38</v>
@@ -1628,19 +1643,19 @@
         <v>41</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="45">
       <c r="A20" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>39</v>
@@ -1652,13 +1667,13 @@
         <v>41</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -1675,7 +1690,9 @@
       <c r="E21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1693,14 +1710,16 @@
       <c r="E22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="45">
       <c r="A23" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>45</v>
@@ -1712,19 +1731,19 @@
         <v>48</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="45">
       <c r="A24" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>46</v>
@@ -1736,13 +1755,13 @@
         <v>48</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -1760,13 +1779,13 @@
         <v>51</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I25" s="1"/>
     </row>
@@ -1784,19 +1803,19 @@
         <v>51</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="30">
       <c r="A27" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>52</v>
@@ -1808,13 +1827,13 @@
         <v>53</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H27" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I27" s="1"/>
     </row>
@@ -1832,10 +1851,10 @@
     </row>
     <row r="29" spans="1:9" ht="30">
       <c r="A29" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>56</v>
@@ -1847,13 +1866,13 @@
         <v>65</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H29" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -1862,7 +1881,7 @@
         <v>45</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>57</v>
@@ -1874,13 +1893,13 @@
         <v>66</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I30" s="1"/>
     </row>
@@ -1898,13 +1917,13 @@
         <v>67</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I31" s="1"/>
     </row>
@@ -1922,13 +1941,13 @@
         <v>68</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I32" s="1"/>
     </row>
@@ -1946,19 +1965,19 @@
         <v>69</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="30">
       <c r="A34" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>61</v>
@@ -1970,13 +1989,13 @@
         <v>70</v>
       </c>
       <c r="F34" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G34" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H34" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I34" s="1"/>
     </row>
@@ -2024,13 +2043,13 @@
         <v>74</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2038,25 +2057,25 @@
         <v>53</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>76</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2064,7 +2083,7 @@
         <v>54</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>75</v>
@@ -2076,13 +2095,13 @@
         <v>77</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="28" customHeight="1">
@@ -2099,7 +2118,7 @@
     </row>
     <row r="41" spans="1:9" ht="30">
       <c r="A41" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>79</v>
@@ -2111,18 +2130,18 @@
         <v>81</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="G41" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H41" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="30">
       <c r="A42" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>82</v>
@@ -2134,13 +2153,13 @@
         <v>84</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="G42" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H42" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2157,13 +2176,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2173,14 +2192,14 @@
     </row>
     <row r="45" spans="1:9" ht="144" customHeight="1">
       <c r="C45" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:9" ht="27" customHeight="1">
       <c r="A46" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B46" s="26"/>
       <c r="C46" s="26"/>

</xml_diff>